<commit_message>
se finalizan todos los escenarios del 4to excel "scotiatrade"
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_004_ScotiatradeTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_004_ScotiatradeTest.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2665F04-FEA0-45D9-8AB8-6F0EE689C158}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8842D6-E4F4-4CF4-9287-20DE77853DFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="233">
   <si>
     <t>Escenario</t>
   </si>
@@ -281,6 +281,505 @@
   <si>
     <t>Rellenamos los campos con una respuesta ya usada||El sistema muestra en pantalla el siguiente mensaje: 
 - Favor de Proporcionar otra pregunta que no haya utilizado</t>
+  </si>
+  <si>
+    <t>SC_004_19_ConsultaCartasConfirmación</t>
+  </si>
+  <si>
+    <t>Ingresar la liga de acceso a ScotiaTrade.||Paso realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Ingresamos un usuario valido y existente.||Paso realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Clickeamos el botón Aceptar.||Click realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Damos Clic en el botón Menú para desplegar las opciones.||Paso reslizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Damos Clic en la opción: 
+-Cartas Confirmación||Paso seleccionado correctamente</t>
+  </si>
+  <si>
+    <t>Ingresamos los datos para consultar las Cartas Confirmación.||Paso realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Seleccionamos el link de alguna carta.||Se muestra la carta confirmación</t>
+  </si>
+  <si>
+    <t>SC_004_20_ConsultaCartasConfirmaciónConToken</t>
+  </si>
+  <si>
+    <t>SC_004_21_CambioDeClaveDeAccesoClaveNuevaIncorrecta</t>
+  </si>
+  <si>
+    <t>Damos Clic en la opción: 
+-Constancias Fiscales||Paso seleccionado correctamente</t>
+  </si>
+  <si>
+    <t>Seleccionamos un ejercicio fiscal.||El sistema muestra las constancias fiscales disponibles.</t>
+  </si>
+  <si>
+    <t>SC_004_22_ConsultaEstadosDeCuenta</t>
+  </si>
+  <si>
+    <t>Damos Clic en la opción: 
+-Navegación superio||Paso seleccionado correctamente</t>
+  </si>
+  <si>
+    <t>Damos Clic en Consulta de Estados de Cuenta.||El Sistema permite la descarga de los correspondietes archivos (PDF y XML).</t>
+  </si>
+  <si>
+    <t>SC_004_23_ConsultaDeMovimientos35Dias</t>
+  </si>
+  <si>
+    <t>Dar Clic en  Movimientos||Paso realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Ingresamos los datos para la consulta (35 días) y selecciónar botón consulta.||El sistema muestra la información de la consulta conforme al look and feel establecido.</t>
+  </si>
+  <si>
+    <t>SC_004_24_ConsultaDeMovimientos35Dias</t>
+  </si>
+  <si>
+    <t>Ingresamos contrato incorrecto para la consulta (35 días).||El Sistema arroja el mensaje N/A</t>
+  </si>
+  <si>
+    <t>SC_004_25_ConsultaDelMóduloConsultaDeMovimientosConMásDe20Registros</t>
+  </si>
+  <si>
+    <t>Ingresamos datos para la consulta y selecciónar botón consulta.||El sistema muestra los primeros 20 registros y el botón Mas Info</t>
+  </si>
+  <si>
+    <t>Hacemos Click en el botón Mas Info.||El Sistema muestra los siguientes 20 registros</t>
+  </si>
+  <si>
+    <t>SC_004_26_Valorización</t>
+  </si>
+  <si>
+    <t>Damos click al botón Consulta de Valorización.||Paso realizado exitasamente.</t>
+  </si>
+  <si>
+    <t>Ingresamos el contrato y damos click al botón Consultar.||El Sistema despliega la información requerida.</t>
+  </si>
+  <si>
+    <t>SC_004_27_Valorización</t>
+  </si>
+  <si>
+    <t>Ingresamos un contrato incorrecto y damos click al botón Consultar.||El Sistema devuelve
+-Error en Consulta de Valorización.</t>
+  </si>
+  <si>
+    <t>SC_004_36_CancelaciónDeOrdenesDeCapitales</t>
+  </si>
+  <si>
+    <t>Seleccionamos la opción de consulta y cancelación de ordenes.||El sistema muestra la pantalla de de consulta y cancelación de ordenes.</t>
+  </si>
+  <si>
+    <t>Damos Click al botón Consulta en la seccion de capitales.||El sistema muestra las ordenes de capitales con el look and feel establecido</t>
+  </si>
+  <si>
+    <t>Seleccionamos una orden y la cancelamos.||El sistema muestra la pantalla de  confirmación de la cancelacion con el look and feel establecido</t>
+  </si>
+  <si>
+    <t>Hacemos Click en el comprobante.||El sistema muestra el comprobante</t>
+  </si>
+  <si>
+    <t>SC_004_37_CancelaciónDeOrdenesDeEfectivo</t>
+  </si>
+  <si>
+    <t>Damos Click al botón Consulta en la seccion de efectivo.||El sistema muestra las ordenes de efectivo con el look and feel establecido</t>
+  </si>
+  <si>
+    <t>SC_004_38_CancelaciónDeOrdenesDeFondos</t>
+  </si>
+  <si>
+    <t>Damos Click al botón Consulta en la seccion de fondos de inversión.||El sistema muestra las ordenes de fondos con el look and feel establecido</t>
+  </si>
+  <si>
+    <t>SC_004_39_ConsultaDeOrdenesDeCapitales</t>
+  </si>
+  <si>
+    <t>SC_004_40_ConsultaDeOrdenesDeEfectivo</t>
+  </si>
+  <si>
+    <t>SC_004_41_ConsultaDeOrdenesFondos</t>
+  </si>
+  <si>
+    <t>SC_004_42_CambioDeClaveDeAccesoNoCapturóNumeroDeUsuario</t>
+  </si>
+  <si>
+    <t>Ingresamos a la URL y damos Click al botón entrar.||El sistema muestra la pantalla de login</t>
+  </si>
+  <si>
+    <t>Hacemos Click en el ícono para cambio de contraseña.||El sistema muestra la pantalla de cambio de contraseña</t>
+  </si>
+  <si>
+    <t>Damos Click al botón aceptar sin capturar numero de usuario.||El sistema notifica el error conforme al look and feel establecido</t>
+  </si>
+  <si>
+    <t>SC_004_43_ConsultaYCancelaciónDeOrdenes</t>
+  </si>
+  <si>
+    <t>Ingresamos a la URL de acceso a ScotiaTrade.||Se muestra la pantalla de "Registro de Usuario" referente a ScotiaTrade</t>
+  </si>
+  <si>
+    <t>Ingresamos un usuario valido y existente, su respectiva "Clave de acceso" valida y click al botón Continuar.||Paso realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Damos Click a la opción "Aceptar".||Click realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Damos Click a la opción "Aceptar".||Se desplegará como panel inicial la pantalla "Información de Mercado".</t>
+  </si>
+  <si>
+    <t>Dar Clic en el menú (Navegación superior).||Se desplegarán las opciones.</t>
+  </si>
+  <si>
+    <t>Damos Clic en Consulta y Cancelación de Ordenes.||El sistema muestra en pantalla los resultados</t>
+  </si>
+  <si>
+    <t>SC_004_44_CapturaDeOrdenesDeMercadoDeCapitalesCompra</t>
+  </si>
+  <si>
+    <t>Damos Click a la opción "Aceptar".||Se desplegará como panel inicial la pantalla "Información de Mercado"</t>
+  </si>
+  <si>
+    <t>Captura de Ordenes del Mercado de Capitales.||El sistema muestra en pantalla los resultados</t>
+  </si>
+  <si>
+    <t>SC_004_45_CapturaDeOrdenesDeMercadoDeCapitalesVenta</t>
+  </si>
+  <si>
+    <t>SC_004_46_OperarMercadoDeCapitalesClaveIncorrecta</t>
+  </si>
+  <si>
+    <t>Ingresamos al aplicativo con el flujo del cp login.||El aplicativo muestra la ventana de información de mercados</t>
+  </si>
+  <si>
+    <t>seleccionamos en el menú de operación la opción "Operar Mercado de capitales".||El aplicativo muestra la pantalla de operación de mercado de capitales</t>
+  </si>
+  <si>
+    <t>Ingresamos una orden de compra y cuando del sistema pida la clave del usuario, ingresamos una clave incorrecta.||El sistema muestra en pantalla el mensaje:
+"La clave proporcionada es inválida. Favor de Verificar".</t>
+  </si>
+  <si>
+    <t>Damos Click en el botón Regresar.||El sistema muestra la pantalla de operación de mercado de capitales</t>
+  </si>
+  <si>
+    <t>Damos Click en el botón Regresar y repetimos el paso anterior pero con una orden de venta.||El sistema muestra en pantalla el mensaje:
+"paso realizado exitosamente".</t>
+  </si>
+  <si>
+    <t>SC_004_47_OperarMercadoDeCapitalesCompraImporteMayorAlDisponible</t>
+  </si>
+  <si>
+    <t>Ingresamos una orden de compra con un importe mayor al disponible.||El sistema muestra en pantalla el mensaje:
+"El saldo disponible no alcanza para operar".</t>
+  </si>
+  <si>
+    <t>SC_004_48_OperarMercadoDeCapitalesVentaSinPosición</t>
+  </si>
+  <si>
+    <t>Ingresamos una orden de venta de una emisora que no se tenga en posición.||El sistema muestra en pantalla el mensaje:
+"El contrato no tiene posición disponible".</t>
+  </si>
+  <si>
+    <t>SC_004_49_OperarEfectivoDeposito</t>
+  </si>
+  <si>
+    <t>Damos Click en Operar Efectivo.||El sistema muestra en pantalla los resultados</t>
+  </si>
+  <si>
+    <t>Capturamos datos para el deposito, damos click en botón aceptar y registramos clave.||El sistema confirma la realización de la operación</t>
+  </si>
+  <si>
+    <t>SC_004_50_OperarEfectivoRetiro</t>
+  </si>
+  <si>
+    <t>Capturamos datos para el deposito, dar click en botón aceptar y registrar clave.||El sistema confirma la realización de la operación</t>
+  </si>
+  <si>
+    <t>Damos click en el botón Aceptar.||El sistema regresa a la pantalla de captura de ordenes de efectivo</t>
+  </si>
+  <si>
+    <t>SC_004_51_OperarEfectivoClaveIncorrecta</t>
+  </si>
+  <si>
+    <t>SC_004_52_OperarEfectivoFueraDeHorario</t>
+  </si>
+  <si>
+    <t>Ingresamos una operación de efectivo y capturamos una orden fuera de horario.||Se debe mostrar mensaje de operacion que esta fuera de horario o en fin de semana</t>
+  </si>
+  <si>
+    <t>Damos click en el botón Regresar.||Se agrega contraseña incorrecta y se da clic en Aceptar.</t>
+  </si>
+  <si>
+    <t>SC_004_53_OperarFondosDeInversiónCompra_FondosCash_Scotia1_ScotiaG</t>
+  </si>
+  <si>
+    <t>seleccionamosdel el menú de operación la opción, "operar fondos de inversión".||El sistema muestra la pantalla de captura de ordenes</t>
+  </si>
+  <si>
+    <t>SC_004_54_OperarFondosDeInversiónCompra_FondosNoCash_Scotia2_Scotilp</t>
+  </si>
+  <si>
+    <t>Capturamos una orden de compra.
+- Ingresar el contrato 77026596
+-Operar con los fondos Scotia1,ScotiaG||El sistema muestra  la confirmación con el icono del comprobante</t>
+  </si>
+  <si>
+    <t>SC_004_55_OperarFondosDeInversiónventa_FondosCash_Scotia1_ScotiaG</t>
+  </si>
+  <si>
+    <t>Capturamos una orden de compra.
+- Ingresar el contrato 77026596
+-Operar con los fondos Scotia2,Scotilip||El sistema muestra  la confirmación con el icono del comprobante</t>
+  </si>
+  <si>
+    <t>SC_004_56_OperarFondosDeInversiónVenta_FondosNoCash_Scotia2_Scotilp</t>
+  </si>
+  <si>
+    <t>Capturamos una orden de compra.
+- Ingresar el contrato 77026596
+-Operar con los fondos Scotia2,Scotilp||El sistema muestra  la confirmación con el icono del comprobante</t>
+  </si>
+  <si>
+    <t>SC_004_57_OperarFondosDeInversión</t>
+  </si>
+  <si>
+    <t>Seleccionamos en el menú la opción "Operar Fondos de Inversión".||Se muestra la pantalla de captura de ordenes con el Look and Feel conforme a especificaciones</t>
+  </si>
+  <si>
+    <t>Capturamos una orden con un importe superior al disponible.||El sistema muentra mensaje en pantalla:
+"El importe debe ser menor o igual al disponible para operar mostrando dicho importe"</t>
+  </si>
+  <si>
+    <t>Capturamos compra por importe menor al disponible y selecionar el botón de confirmar.||El sistema solicita el pasword, procesa la orden y devuelve pantalla de confirmación. Se muestran los elementos del Look and Feel de manera correcta</t>
+  </si>
+  <si>
+    <t>SC_004_58_ConsultaDelBannerUnosDosYConoceMás</t>
+  </si>
+  <si>
+    <t>Esperamos solo un poco de tiempo.||el sistema presenta la pantalla de login</t>
+  </si>
+  <si>
+    <t>Damos Clic en el botón Conoce Más.||El sistema muestra en pantalla la página de ver mas detalle del Contrato de Inversión de Scotiabank</t>
+  </si>
+  <si>
+    <t>SC_004_59_OperarFondosDeInversión</t>
+  </si>
+  <si>
+    <t>Capturar orden con fondo no permitido para el contrato.||El sistema muestra en pantalla el mensaje:
+"el usuario no puede operar el fondo"</t>
+  </si>
+  <si>
+    <t>Damos Click en el botón Regresar.||Se muestra pantalla de captura de ordenes de fondos de inversión</t>
+  </si>
+  <si>
+    <t>SC_004_60_OperarFondosDeInversión</t>
+  </si>
+  <si>
+    <t>Capturamos una orden con importe mayor al disponible.||Se muestra pantalla con el aviso de que el usuario no puede operar el fondo</t>
+  </si>
+  <si>
+    <t>SC_004_61_OperarFondosDeInversión</t>
+  </si>
+  <si>
+    <t>Capturamos una orden de venta de un fondo que no se tiene en posición.||Se muestra pantalla con el aviso</t>
+  </si>
+  <si>
+    <t>SC_004_62_CambioDeMail</t>
+  </si>
+  <si>
+    <t>Ingresamos el  N° Cliente, Clave de acceso y Clic en el botón Continuar.||Se muestra la información de Frase e Imagen del usuario</t>
+  </si>
+  <si>
+    <t>Una vez verificado Información de Frase e Imagen, Damos Clic en aceptar.||El sistema muestra un mensaje de bienvenida  con el nombre del cliente y fecha de ultima sesión</t>
+  </si>
+  <si>
+    <t>Presionamos el botón "Aceptar" del mensaje.||Se abre una nueva ventana con la información de Mercado de Infosel.</t>
+  </si>
+  <si>
+    <t>Damos Click en el botón Cambio de Mail.||El sistema muestra la pantalla "Cambio de Mail"</t>
+  </si>
+  <si>
+    <t>Ingresamos los nuevos datos y damos click en el botón Modificar.||Paso realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Dejamos en blanco el display del dispositivo e-Llave y damos click al botón Aceptar.||El sistema muestra en pantalla el mensaje:
+ "Sus registros han sido dados de alta"</t>
+  </si>
+  <si>
+    <t>Damos click en el botón "Aceptar".||Se muestra la confirmación del cambio y regresa a la pantalla inicial "Cambio de Mail".</t>
+  </si>
+  <si>
+    <t>SC_004_63_CambioDeMail</t>
+  </si>
+  <si>
+    <t>Damos Click en el botón Cambio de Pregunta.||El sistema muestra la pantalla "Cambio de Pregunta Secreta"</t>
+  </si>
+  <si>
+    <t>SC_004_64_ConsultaCartasConfirmación</t>
+  </si>
+  <si>
+    <t>Ingresamos los datos requeridos y damos click en el botón Buscar.||Paso realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Capturamos los dígitos del display del dispositivo e-Llave y presionamos el botón Aceptar.||El sistema muestra una tabla con las cartas confirmación resultantes de la búsqueda.</t>
+  </si>
+  <si>
+    <t>Seleccionamos el número de carta confirmación a consultar.||Se muestra una pantalla de "Descarga de Archi vos" con el archivo en formato PDF y las opciones: "Abrir"
+"Guardar"
+"Cancelar".</t>
+  </si>
+  <si>
+    <t>Damos Click la opción "Abrir" de la pantalla de Descarga.||Se visualiza la Carta Confirmación seleccionada en formato PDF</t>
+  </si>
+  <si>
+    <t>SC_004_65_ConsultaEstadoDeCuentaPDF</t>
+  </si>
+  <si>
+    <t>Ingresamos a la URL de acceso a ScotiaTrade.||Mostrará la pagina donde se firmará el usuario</t>
+  </si>
+  <si>
+    <t>Damos Click en el botón Consulta Estados Cuenta.||El sistema muestra la pantalla "Consulta Estados de Cuenta"</t>
+  </si>
+  <si>
+    <t>Ingresamos los datos requeridos y damos click en el botón Consultar.||Paso realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Capturamos el código de la e-llave y presionamos el botón Aceptar.||Se muestra una pantalla de "Descarga de Archi vos" con el archivo en formato PDF y las opciones:
+"Abrir"
+"Guardar"
+"Cancelar".</t>
+  </si>
+  <si>
+    <t>Presionamos la opción Abrir de la pantalla de Descarga.||Se visualiza el Estado de Cuenta indicado en formato PDF.</t>
+  </si>
+  <si>
+    <t>SC_004_66_ConsultaEstadoDeCuentaXML</t>
+  </si>
+  <si>
+    <t>Capturamos el código de la e-llave y presionamos el botón Aceptar.||Se muestra una pantalla de "XML Estado de Cuenta generado" con las opciones:
+"Abrir"
+"Guardar"
+"Cancelar".</t>
+  </si>
+  <si>
+    <t>Presionamos el botón Abrir de la pantalla "XML Estado de Cuenta generado".||Se abrira una ventana donde se realiza la Descarga del XML</t>
+  </si>
+  <si>
+    <t>Damos doble clic en el archivo XML Descargado.||Se muestra la información del Estado de Cuenta en formato XML</t>
+  </si>
+  <si>
+    <t>SC_004_30_XXX</t>
+  </si>
+  <si>
+    <t>SC_004_31_LoginNuevoUsuario</t>
+  </si>
+  <si>
+    <t>Ingresamos a la URL de acceso a ScotiaTrade.||El sistema muestra la pantalla referente a ScotiaTrade</t>
+  </si>
+  <si>
+    <t>Damos Clic en el botón entrar.||Click realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Ingresamos los datos requeridos y damos click en el botón Continuar.||Paso realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Ingresamos la información para el cambio de clave.||Paso realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Damos clic al botón Aceptar.||Se mostrara el cambio de pregunta Secreta</t>
+  </si>
+  <si>
+    <t>Ingresamos la información para el cambio de pregunta Serceta.||Paso realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Damos clic al botón Aceptar.||Se mostrara el mensaje confirmando el cambio de clave</t>
+  </si>
+  <si>
+    <t>El sistema muestra el login de Scotiatrade.||Paso realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Ingresamos nuevos datos para cambio de imagen.||El sistema confirma del cambio de imagen</t>
+  </si>
+  <si>
+    <t>SC_004_32_Login</t>
+  </si>
+  <si>
+    <t>Damos Clic en la opción Aceptar.||El Sistema muestra en pantalla mensaje con información del cliente.</t>
+  </si>
+  <si>
+    <t>Damos Clic en la opción Aceptar.||El sistema despliega en pantalla información de Mercados</t>
+  </si>
+  <si>
+    <t>SC_004_33_LoginClaveIncorrecta</t>
+  </si>
+  <si>
+    <t>Ingresamos un Usuario valido y Clave incorrecta.||El sistema alerta que el usuario y/o clave es incorrecta</t>
+  </si>
+  <si>
+    <t>SC_004_34_LoginUsuarioIncorrecto</t>
+  </si>
+  <si>
+    <t>Ingresamos un Usuario no valido (menos de 6 dígitos).||El sistema alerta que el usuario debe tener 6 dígitos</t>
+  </si>
+  <si>
+    <t>SC_004_35_OlvidoDeContraseña</t>
+  </si>
+  <si>
+    <t>Ingresamos a la liga y seleccionar el botón entrar.||El sistema muestra la pantalla de login.</t>
+  </si>
+  <si>
+    <t>Hacemos Click en el ícono para cambio de contraseña.||El sistema muestra la pantalla de busqueda de pregunta personal</t>
+  </si>
+  <si>
+    <t>Ingresamos el número de Usuario y damos click en el botón Buscar.||El sistema muestra la pregunta secreta y el campo para la respuesta</t>
+  </si>
+  <si>
+    <t>Ingresamos la respuesta.||El sistema mustra la pantalla para cambio de contraseña.</t>
+  </si>
+  <si>
+    <t>Ingresamos la información para el cambio.||El sistema confirma el  cambio.</t>
+  </si>
+  <si>
+    <t>SC_004_28_GuíaDiaria</t>
+  </si>
+  <si>
+    <t>Ingresamos a la liga de acceso a ScotiaTrade.||Se muestra la pantalla referente a ScotiaTrade</t>
+  </si>
+  <si>
+    <t>Damos clic al botón Entrar.||Se muestra el Login Scotia Trade con los campos de No. de Usuario y Clave acceso</t>
+  </si>
+  <si>
+    <t>Ingresamos Usuario y Contraseña Valido y damos Clic en el botón Continuar.||Paso realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Damos Clic en el Botón Aceptar.||Click realizado exitosamente</t>
+  </si>
+  <si>
+    <t>Damos Clic en el Botón Cerrar.||El sistema muestra la pantalla Principal</t>
+  </si>
+  <si>
+    <t>Damos Clic en la Opción Menú.||El sistema debe desplegar el Menu.</t>
+  </si>
+  <si>
+    <t>SC_004_29_InformaciónDeMercados</t>
+  </si>
+  <si>
+    <t>Seleccionamos la Opcion de "Guia Diaria".||El sistema nos debe mostrar en otra pantalla la Guia diaria.</t>
+  </si>
+  <si>
+    <t>Seleccionamos la opción de "Información de Mercado".||El sistema muestra en pantalla la información requerida</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Seleccionamos la opción de "Manual de Operacion".||El sistema muestra en pantalla la información requerida</t>
   </si>
 </sst>
 </file>
@@ -322,7 +821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -330,11 +829,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,22 +1127,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
     <col min="9" max="9" width="42.85546875" customWidth="1"/>
     <col min="10" max="10" width="39.42578125" customWidth="1"/>
     <col min="11" max="11" width="38.5703125" customWidth="1"/>
@@ -689,7 +1200,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1"/>
@@ -718,8 +1229,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2"/>
@@ -748,8 +1259,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1"/>
@@ -779,7 +1290,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1"/>
@@ -812,7 +1323,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1"/>
@@ -844,8 +1355,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1"/>
@@ -877,8 +1388,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1"/>
@@ -899,98 +1410,98 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>47</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>50</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1012,222 +1523,1512 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:15" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+    </row>
+    <row r="39" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+    </row>
+    <row r="40" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+    </row>
+    <row r="41" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+    </row>
+    <row r="42" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+    </row>
+    <row r="43" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+    </row>
+    <row r="44" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+    </row>
+    <row r="45" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+    </row>
+    <row r="46" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+    </row>
+    <row r="47" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+    </row>
+    <row r="48" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
+      <c r="P48" s="6"/>
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="6"/>
+    </row>
+    <row r="49" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="6"/>
+    </row>
+    <row r="51" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="6"/>
+      <c r="Q51" s="6"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="6"/>
+    </row>
+    <row r="52" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+    </row>
+    <row r="53" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+    </row>
+    <row r="54" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>